<commit_message>
kb config and template done
</commit_message>
<xml_diff>
--- a/invoice_gen/TEMPLATE/KB.xlsx
+++ b/invoice_gen/TEMPLATE/KB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPZ031127\Desktop\automate invoice\invoice_gen\TEMPLATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5809B65D-0BB3-4893-8FDC-0989FB28620E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0566F2C1-74A2-42A2-95B3-8D79E3A3A1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contract" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="56">
   <si>
     <t xml:space="preserve">CALIFOR UPHOLSTERY MATERIALS CO., LTD.
 XIN BAVET SEZ, Road No. 316A, Trapeang Bon and  Prey Kokir  Villages, Prey Kokir Commune, Chantrea District, Svay Rieng Province, Kingdom of Cambodia.
@@ -76,12 +76,6 @@
   </si>
   <si>
     <t>Place of Departure</t>
-  </si>
-  <si>
-    <t>KB25010</t>
-  </si>
-  <si>
-    <t>16/5/2025</t>
   </si>
   <si>
     <t>BAVET,CAMBOIDA</t>
@@ -255,12 +249,6 @@
     <t>PACKING LIST</t>
   </si>
   <si>
-    <t xml:space="preserve">CLF2025-146                   </t>
-  </si>
-  <si>
-    <t>KB25011</t>
-  </si>
-  <si>
     <t>BINH DUONG</t>
   </si>
   <si>
@@ -284,6 +272,15 @@
                                           /BANK OF CHINA PHNOM PENH BRANCH</t>
     </r>
   </si>
+  <si>
+    <t>JFTIME</t>
+  </si>
+  <si>
+    <t>JFREF</t>
+  </si>
+  <si>
+    <t>JFINV</t>
+  </si>
 </sst>
 </file>
 
@@ -291,8 +288,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
-    <numFmt numFmtId="166" formatCode="[$USD]\ #,##0.00;[$USD]\ \-#,##0.00"/>
-    <numFmt numFmtId="167" formatCode="yyyy/mm/dd;@"/>
+    <numFmt numFmtId="165" formatCode="[$USD]\ #,##0.00;[$USD]\ \-#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -469,7 +466,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -681,13 +678,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -786,100 +819,85 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="22" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="22" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="22" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="22" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="21" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="21" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="18" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="18" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="18" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -912,6 +930,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1221,10 +1275,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18" customHeight="1"/>
@@ -1237,208 +1291,306 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="35.1" customHeight="1">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="57" t="s">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="58"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="53"/>
     </row>
     <row r="2" spans="1:10" ht="35.1" customHeight="1">
-      <c r="A2" s="68"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="59" t="s">
+      <c r="A2" s="63"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="60"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="55"/>
     </row>
     <row r="3" spans="1:10" s="39" customFormat="1" ht="15" customHeight="1">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50" t="s">
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="51"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="46"/>
     </row>
     <row r="4" spans="1:10" ht="99.95" customHeight="1">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="62"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="63" t="s">
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="65"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="60"/>
     </row>
     <row r="5" spans="1:10" s="39" customFormat="1" ht="14.1" customHeight="1">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50" t="s">
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50" t="s">
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="51"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="46"/>
     </row>
     <row r="6" spans="1:10" ht="23.1" customHeight="1">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="54"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="53" t="s">
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="50"/>
+    </row>
+    <row r="7" spans="1:10" s="39" customFormat="1" ht="14.1" customHeight="1">
+      <c r="A7" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="54" t="s">
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="55"/>
-    </row>
-    <row r="7" spans="1:10" s="39" customFormat="1" ht="14.1" customHeight="1">
-      <c r="A7" s="49" t="s">
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50" t="s">
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="46"/>
+    </row>
+    <row r="8" spans="1:10" ht="23.1" customHeight="1">
+      <c r="A8" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="51"/>
-    </row>
-    <row r="8" spans="1:10" ht="23.1" customHeight="1">
-      <c r="A8" s="56" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="54"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="54" t="str">
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49" t="str">
         <f>[1]INV!D8</f>
         <v>T/T</v>
       </c>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="54" t="s">
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="50"/>
+    </row>
+    <row r="9" spans="1:10" s="39" customFormat="1" ht="14.1" customHeight="1">
+      <c r="A9" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="54"/>
-      <c r="I8" s="54"/>
-      <c r="J8" s="55"/>
-    </row>
-    <row r="9" spans="1:10" s="39" customFormat="1" ht="14.1" customHeight="1">
-      <c r="A9" s="49" t="s">
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50" t="s">
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="46"/>
+    </row>
+    <row r="10" spans="1:10" ht="23.1" customHeight="1">
+      <c r="A10" s="47" t="str">
+        <f>D6</f>
+        <v>JFTIME</v>
+      </c>
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50" t="s">
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="50"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="51"/>
-    </row>
-    <row r="10" spans="1:10" ht="23.1" customHeight="1">
-      <c r="A10" s="52" t="str">
-        <f>D6</f>
-        <v>16/5/2025</v>
-      </c>
-      <c r="B10" s="53"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="54" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
-      <c r="G10" s="54" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" s="54"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="55"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="50"/>
     </row>
     <row r="11" spans="1:10" s="39" customFormat="1" ht="14.1" customHeight="1"/>
     <row r="12" spans="1:10" s="39" customFormat="1" ht="24.95" customHeight="1"/>
     <row r="13" spans="1:10" s="39" customFormat="1" ht="24.95" customHeight="1"/>
     <row r="14" spans="1:10" ht="23.1" customHeight="1"/>
-    <row r="15" spans="1:10" s="39" customFormat="1" ht="14.1" customHeight="1">
-      <c r="A15" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
-      <c r="J15" s="43"/>
-    </row>
-    <row r="16" spans="1:10" ht="115.5" customHeight="1">
-      <c r="A16" s="44"/>
-      <c r="B16" s="45"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="45"/>
-      <c r="J16" s="48"/>
+    <row r="15" spans="1:10" s="39" customFormat="1" ht="14.1" customHeight="1"/>
+    <row r="16" spans="1:10" ht="115.5" customHeight="1"/>
+    <row r="19" spans="1:10" ht="18" customHeight="1">
+      <c r="A19" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="43"/>
+    </row>
+    <row r="20" spans="1:10" ht="18" customHeight="1">
+      <c r="A20" s="80"/>
+      <c r="B20" s="77"/>
+      <c r="C20" s="77"/>
+      <c r="D20" s="77"/>
+      <c r="E20" s="86"/>
+      <c r="F20" s="85"/>
+      <c r="G20" s="79"/>
+      <c r="H20" s="79"/>
+      <c r="I20" s="79"/>
+      <c r="J20" s="82"/>
+    </row>
+    <row r="21" spans="1:10" ht="18" customHeight="1">
+      <c r="A21" s="80"/>
+      <c r="B21" s="77"/>
+      <c r="C21" s="77"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="86"/>
+      <c r="F21" s="85"/>
+      <c r="G21" s="79"/>
+      <c r="H21" s="79"/>
+      <c r="I21" s="79"/>
+      <c r="J21" s="82"/>
+    </row>
+    <row r="22" spans="1:10" ht="18" customHeight="1">
+      <c r="A22" s="80"/>
+      <c r="B22" s="77"/>
+      <c r="C22" s="77"/>
+      <c r="D22" s="77"/>
+      <c r="E22" s="86"/>
+      <c r="F22" s="85"/>
+      <c r="G22" s="79"/>
+      <c r="H22" s="79"/>
+      <c r="I22" s="79"/>
+      <c r="J22" s="82"/>
+    </row>
+    <row r="23" spans="1:10" ht="18" customHeight="1">
+      <c r="A23" s="80"/>
+      <c r="B23" s="77"/>
+      <c r="C23" s="77"/>
+      <c r="D23" s="77"/>
+      <c r="E23" s="86"/>
+      <c r="F23" s="85"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="79"/>
+      <c r="I23" s="79"/>
+      <c r="J23" s="82"/>
+    </row>
+    <row r="24" spans="1:10" ht="18" customHeight="1">
+      <c r="A24" s="80"/>
+      <c r="B24" s="77"/>
+      <c r="C24" s="77"/>
+      <c r="D24" s="77"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="85"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="79"/>
+      <c r="J24" s="82"/>
+    </row>
+    <row r="25" spans="1:10" ht="18" customHeight="1">
+      <c r="A25" s="80"/>
+      <c r="B25" s="77"/>
+      <c r="C25" s="77"/>
+      <c r="D25" s="77"/>
+      <c r="E25" s="86"/>
+      <c r="F25" s="85"/>
+      <c r="G25" s="79"/>
+      <c r="H25" s="79"/>
+      <c r="I25" s="79"/>
+      <c r="J25" s="82"/>
+    </row>
+    <row r="26" spans="1:10" ht="18" customHeight="1">
+      <c r="A26" s="80"/>
+      <c r="B26" s="77"/>
+      <c r="C26" s="77"/>
+      <c r="D26" s="77"/>
+      <c r="E26" s="86"/>
+      <c r="F26" s="85"/>
+      <c r="G26" s="79"/>
+      <c r="H26" s="79"/>
+      <c r="I26" s="79"/>
+      <c r="J26" s="82"/>
+    </row>
+    <row r="27" spans="1:10" ht="18" customHeight="1">
+      <c r="A27" s="80"/>
+      <c r="B27" s="77"/>
+      <c r="C27" s="77"/>
+      <c r="D27" s="77"/>
+      <c r="E27" s="86"/>
+      <c r="F27" s="85"/>
+      <c r="G27" s="79"/>
+      <c r="H27" s="79"/>
+      <c r="I27" s="79"/>
+      <c r="J27" s="82"/>
+    </row>
+    <row r="28" spans="1:10" ht="18" customHeight="1" thickBot="1">
+      <c r="A28" s="76"/>
+      <c r="B28" s="81"/>
+      <c r="C28" s="81"/>
+      <c r="D28" s="81"/>
+      <c r="E28" s="87"/>
+      <c r="F28" s="78"/>
+      <c r="G28" s="83"/>
+      <c r="H28" s="83"/>
+      <c r="I28" s="83"/>
+      <c r="J28" s="84"/>
     </row>
   </sheetData>
   <mergeCells count="29">
@@ -1461,16 +1613,16 @@
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="D8:F8"/>
     <mergeCell ref="G8:J8"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="F19:J19"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="G9:J9"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="G10:J10"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="F15:J15"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="F16:J16"/>
+    <mergeCell ref="A20:E28"/>
+    <mergeCell ref="F20:J28"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait"/>
@@ -1482,8 +1634,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A14" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15"/>
@@ -1503,70 +1655,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="38.25" customHeight="1">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="70" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+    </row>
+    <row r="2" spans="1:7" ht="24" customHeight="1">
+      <c r="A2" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+    </row>
+    <row r="3" spans="1:7" ht="17.25" customHeight="1">
+      <c r="A3" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-    </row>
-    <row r="2" spans="1:7" ht="24" customHeight="1">
-      <c r="A2" s="76" t="s">
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+    </row>
+    <row r="4" spans="1:7" ht="17.25" customHeight="1">
+      <c r="A4" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-    </row>
-    <row r="3" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A3" s="77" t="s">
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
+    </row>
+    <row r="5" spans="1:7" ht="25.5" customHeight="1">
+      <c r="A5" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="77"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-    </row>
-    <row r="4" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A4" s="77" t="s">
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+    </row>
+    <row r="6" spans="1:7" ht="83.25" customHeight="1">
+      <c r="A6" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="77"/>
-    </row>
-    <row r="5" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A5" s="78" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-    </row>
-    <row r="6" spans="1:7" ht="83.25" customHeight="1">
-      <c r="A6" s="71" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="71"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
+      <c r="B6" s="66"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
     </row>
     <row r="7" spans="1:7" ht="14.25" customHeight="1">
       <c r="A7" s="5"/>
@@ -1575,57 +1727,54 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="5" t="str">
-        <f>'Packing list'!I7</f>
-        <v xml:space="preserve">CLF2025-146                   </v>
+        <v>28</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1">
       <c r="A8" s="33" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
       <c r="E8" s="8"/>
       <c r="F8" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="14" t="str">
-        <f>'Packing list'!I8</f>
-        <v>KB25011</v>
+        <v>30</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="21" customHeight="1">
       <c r="A9" s="10"/>
       <c r="B9" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="32">
-        <f>'Packing list'!I9</f>
-        <v>44338</v>
+        <v>32</v>
+      </c>
+      <c r="G9" s="32" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="22.5" customHeight="1">
       <c r="A10" s="10"/>
       <c r="B10" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
       <c r="F10" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G10" s="16" t="str">
         <f>'Packing list'!I10</f>
@@ -1635,7 +1784,7 @@
     <row r="11" spans="1:7" ht="20.25" customHeight="1">
       <c r="A11" s="10"/>
       <c r="B11" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -1663,10 +1812,10 @@
     </row>
     <row r="14" spans="1:7" ht="25.5" customHeight="1">
       <c r="A14" s="33" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
@@ -1676,7 +1825,7 @@
     <row r="15" spans="1:7" ht="25.5" customHeight="1">
       <c r="A15" s="10"/>
       <c r="B15" s="16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
@@ -1686,7 +1835,7 @@
     <row r="16" spans="1:7" ht="25.5" customHeight="1">
       <c r="A16" s="10"/>
       <c r="B16" s="16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
@@ -1696,7 +1845,7 @@
     <row r="17" spans="1:7" ht="25.5" customHeight="1">
       <c r="A17" s="10"/>
       <c r="B17" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -1705,10 +1854,10 @@
     </row>
     <row r="18" spans="1:7" ht="27.75" customHeight="1">
       <c r="A18" s="20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -1741,11 +1890,11 @@
       <c r="G23" s="19"/>
     </row>
     <row r="24" spans="1:7" ht="42" customHeight="1">
-      <c r="A24" s="72" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="72"/>
-      <c r="C24" s="72"/>
+      <c r="A24" s="67" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="67"/>
+      <c r="C24" s="67"/>
       <c r="D24" s="23"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
@@ -1753,61 +1902,61 @@
     </row>
     <row r="25" spans="1:7" ht="61.5" customHeight="1">
       <c r="A25" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="73" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="73"/>
+        <v>43</v>
+      </c>
+      <c r="B25" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="68"/>
       <c r="D25" s="26"/>
       <c r="E25" s="26"/>
       <c r="F25" s="5"/>
       <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7" ht="42" customHeight="1">
-      <c r="A26" s="74" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="74"/>
-      <c r="C26" s="74"/>
+      <c r="A26" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="69"/>
+      <c r="C26" s="69"/>
       <c r="D26" s="27"/>
       <c r="E26" s="27"/>
       <c r="F26" s="27"/>
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:7" ht="24.75" customHeight="1">
-      <c r="A27" s="70" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="70"/>
-      <c r="C27" s="70"/>
-      <c r="D27" s="70"/>
-      <c r="E27" s="70"/>
-      <c r="F27" s="70"/>
-      <c r="G27" s="70"/>
+      <c r="A27" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="65"/>
+      <c r="C27" s="65"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="65"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="65"/>
     </row>
     <row r="28" spans="1:7" s="2" customFormat="1" ht="27" customHeight="1">
-      <c r="A28" s="70" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="70"/>
-      <c r="C28" s="70"/>
-      <c r="D28" s="70"/>
-      <c r="E28" s="70"/>
-      <c r="F28" s="70"/>
-      <c r="G28" s="70"/>
+      <c r="A28" s="65" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="65"/>
+      <c r="C28" s="65"/>
+      <c r="D28" s="65"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="65"/>
     </row>
     <row r="29" spans="1:7" ht="42" customHeight="1">
       <c r="E29" s="10"/>
       <c r="F29" s="12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G29" s="4"/>
     </row>
     <row r="30" spans="1:7" ht="24" customHeight="1">
       <c r="E30" s="5"/>
       <c r="F30" s="29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="69.75" customHeight="1">
@@ -1817,13 +1966,13 @@
     <row r="32" spans="1:7" ht="42" customHeight="1">
       <c r="E32" s="5"/>
       <c r="F32" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="5:7" ht="53.1" customHeight="1">
       <c r="E33" s="5"/>
       <c r="F33" s="37" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G33" s="6"/>
     </row>
@@ -1876,8 +2025,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A12" zoomScale="85" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15"/>
@@ -1902,92 +2051,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="38.25" customHeight="1">
-      <c r="A1" s="75" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
+      <c r="A1" s="70" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
       <c r="J1" s="30"/>
       <c r="K1" s="30"/>
     </row>
     <row r="2" spans="1:11" ht="24" customHeight="1">
-      <c r="A2" s="76" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
+      <c r="A2" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:11" ht="25.5" customHeight="1">
-      <c r="A3" s="77" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="77"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
+      <c r="A3" s="72" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
       <c r="J3" s="28"/>
       <c r="K3" s="28"/>
     </row>
     <row r="4" spans="1:11" ht="25.5" customHeight="1">
-      <c r="A4" s="80" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="80"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="80"/>
+      <c r="A4" s="75" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
       <c r="J4" s="28"/>
       <c r="K4" s="28"/>
     </row>
     <row r="5" spans="1:11" ht="25.5" customHeight="1">
-      <c r="A5" s="78" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
+      <c r="A5" s="73" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
       <c r="J5" s="28"/>
       <c r="K5" s="28"/>
     </row>
     <row r="6" spans="1:11" ht="54" customHeight="1">
-      <c r="A6" s="71" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="71"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="71"/>
+      <c r="A6" s="66" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="66"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="66"/>
       <c r="J6" s="31"/>
       <c r="K6" s="31"/>
     </row>
@@ -2000,65 +2149,65 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="30" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="21" customHeight="1">
       <c r="A9" s="5"/>
       <c r="B9" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="I9" s="32">
-        <v>44338</v>
+        <v>32</v>
+      </c>
+      <c r="I9" s="32" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="22.5" customHeight="1">
       <c r="A10" s="5"/>
       <c r="B10" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:11" ht="20.25" customHeight="1">
       <c r="A11" s="5"/>
       <c r="B11" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
@@ -2084,10 +2233,10 @@
     </row>
     <row r="13" spans="1:11" ht="25.5" customHeight="1">
       <c r="A13" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
@@ -2099,7 +2248,7 @@
     <row r="14" spans="1:11" ht="25.5" customHeight="1">
       <c r="A14" s="5"/>
       <c r="B14" s="16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
@@ -2111,7 +2260,7 @@
     <row r="15" spans="1:11" ht="25.5" customHeight="1">
       <c r="A15" s="5"/>
       <c r="B15" s="16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
@@ -2123,7 +2272,7 @@
     <row r="16" spans="1:11" ht="25.5" customHeight="1">
       <c r="A16" s="5"/>
       <c r="B16" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
@@ -2134,10 +2283,10 @@
     </row>
     <row r="17" spans="1:12" ht="27.75" customHeight="1">
       <c r="A17" s="20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -2170,11 +2319,11 @@
       <c r="I21" s="9"/>
     </row>
     <row r="22" spans="1:12" ht="48" customHeight="1">
-      <c r="A22" s="72" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="72"/>
-      <c r="C22" s="72"/>
+      <c r="A22" s="67" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="67"/>
+      <c r="C22" s="67"/>
       <c r="D22" s="24"/>
       <c r="E22" s="23"/>
       <c r="F22" s="5"/>
@@ -2187,12 +2336,12 @@
     </row>
     <row r="23" spans="1:12" ht="59.1" customHeight="1">
       <c r="A23" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="73" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="73"/>
+        <v>43</v>
+      </c>
+      <c r="B23" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="68"/>
       <c r="D23" s="26"/>
       <c r="E23" s="26"/>
       <c r="F23" s="26"/>
@@ -2204,11 +2353,11 @@
       <c r="L23" s="12"/>
     </row>
     <row r="24" spans="1:12" ht="48" customHeight="1">
-      <c r="A24" s="74" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24" s="74"/>
-      <c r="C24" s="74"/>
+      <c r="A24" s="69" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="69"/>
+      <c r="C24" s="69"/>
       <c r="D24" s="27"/>
       <c r="E24" s="27"/>
       <c r="F24" s="27"/>
@@ -2220,40 +2369,40 @@
       <c r="L24" s="12"/>
     </row>
     <row r="25" spans="1:12" ht="48" customHeight="1">
-      <c r="A25" s="70" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="70"/>
-      <c r="C25" s="70"/>
-      <c r="D25" s="70"/>
-      <c r="E25" s="70"/>
-      <c r="F25" s="70"/>
-      <c r="G25" s="70"/>
-      <c r="H25" s="70"/>
-      <c r="I25" s="70"/>
-      <c r="J25" s="70"/>
-      <c r="K25" s="70"/>
+      <c r="A25" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="65"/>
+      <c r="C25" s="65"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="65"/>
+      <c r="H25" s="65"/>
+      <c r="I25" s="65"/>
+      <c r="J25" s="65"/>
+      <c r="K25" s="65"/>
     </row>
     <row r="26" spans="1:12" s="2" customFormat="1" ht="48" customHeight="1">
-      <c r="A26" s="70" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="70"/>
-      <c r="C26" s="70"/>
-      <c r="D26" s="70"/>
-      <c r="E26" s="70"/>
-      <c r="F26" s="70"/>
-      <c r="G26" s="70"/>
-      <c r="H26" s="70"/>
-      <c r="I26" s="70"/>
-      <c r="J26" s="70"/>
-      <c r="K26" s="70"/>
+      <c r="A26" s="65" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="65"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="65"/>
+      <c r="G26" s="65"/>
+      <c r="H26" s="65"/>
+      <c r="I26" s="65"/>
+      <c r="J26" s="65"/>
+      <c r="K26" s="65"/>
     </row>
     <row r="27" spans="1:12" ht="42" customHeight="1">
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I27" s="4"/>
     </row>
@@ -2271,10 +2420,10 @@
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J30" s="79"/>
-      <c r="K30" s="79"/>
+        <v>49</v>
+      </c>
+      <c r="J30" s="74"/>
+      <c r="K30" s="74"/>
     </row>
     <row r="31" spans="1:12" ht="53.1" customHeight="1">
       <c r="F31" s="5"/>
@@ -2310,13 +2459,13 @@
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A4:I4"/>
     <mergeCell ref="A5:I5"/>
+    <mergeCell ref="A26:K26"/>
+    <mergeCell ref="J30:K30"/>
     <mergeCell ref="A6:I6"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="A24:C24"/>
     <mergeCell ref="A25:K25"/>
-    <mergeCell ref="A26:K26"/>
-    <mergeCell ref="J30:K30"/>
   </mergeCells>
   <conditionalFormatting sqref="N22:N34">
     <cfRule type="duplicateValues" priority="1" stopIfTrue="1"/>

</xml_diff>